<commit_message>
Actualización previa a corregir y amplicar tipos de datos
</commit_message>
<xml_diff>
--- a/summary.xlsx
+++ b/summary.xlsx
@@ -426,7 +426,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:P8"/>
+  <dimension ref="A1:P10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -519,7 +519,7 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>ID</t>
+          <t>case_id</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
@@ -528,52 +528,52 @@
         </is>
       </c>
       <c r="C2" t="n">
-        <v>9512</v>
+        <v>318438</v>
       </c>
       <c r="D2" t="n">
         <v>0</v>
       </c>
       <c r="E2" t="n">
-        <v>9512</v>
+        <v>318438</v>
       </c>
       <c r="F2" t="n">
-        <v>6308943</v>
+        <v>1</v>
       </c>
       <c r="G2" t="n">
         <v>1</v>
       </c>
       <c r="H2" t="n">
-        <v>0.01</v>
+        <v>0</v>
       </c>
       <c r="I2" t="n">
-        <v>8210750.886459209</v>
+        <v>159219.5</v>
       </c>
       <c r="J2" t="n">
-        <v>1099345.770765004</v>
+        <v>91925.276847557</v>
       </c>
       <c r="K2" t="n">
-        <v>1208561123698.9</v>
+        <v>8450256523.5</v>
       </c>
       <c r="L2" t="n">
-        <v>6308943</v>
+        <v>1</v>
       </c>
       <c r="M2" t="n">
-        <v>7227208.75</v>
+        <v>79610.25</v>
       </c>
       <c r="N2" t="n">
-        <v>8342317</v>
+        <v>159219.5</v>
       </c>
       <c r="O2" t="n">
-        <v>9160217.75</v>
+        <v>238828.75</v>
       </c>
       <c r="P2" t="n">
-        <v>9987369</v>
+        <v>318438</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>CLIENTEPORCAMPA•AEMAIL</t>
+          <t>Hospital_code</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
@@ -582,52 +582,52 @@
         </is>
       </c>
       <c r="C3" t="n">
-        <v>9512</v>
+        <v>318438</v>
       </c>
       <c r="D3" t="n">
         <v>0</v>
       </c>
       <c r="E3" t="n">
-        <v>2</v>
+        <v>32</v>
       </c>
       <c r="F3" t="n">
-        <v>0</v>
+        <v>26</v>
       </c>
       <c r="G3" t="n">
-        <v>8717</v>
+        <v>33076</v>
       </c>
       <c r="H3" t="n">
-        <v>91.64</v>
+        <v>10.39</v>
       </c>
       <c r="I3" t="n">
-        <v>0.08357863751051303</v>
+        <v>18.31884071624618</v>
       </c>
       <c r="J3" t="n">
-        <v>0.2767694021834417</v>
+        <v>8.633754885795049</v>
       </c>
       <c r="K3" t="n">
-        <v>0.07660130198497972</v>
+        <v>74.54172342798988</v>
       </c>
       <c r="L3" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M3" t="n">
-        <v>0</v>
+        <v>11</v>
       </c>
       <c r="N3" t="n">
-        <v>0</v>
+        <v>19</v>
       </c>
       <c r="O3" t="n">
-        <v>0</v>
+        <v>26</v>
       </c>
       <c r="P3" t="n">
-        <v>1</v>
+        <v>32</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>DIASCLIENTE</t>
+          <t>City_Code_Hospital</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
@@ -636,52 +636,52 @@
         </is>
       </c>
       <c r="C4" t="n">
-        <v>9512</v>
+        <v>318438</v>
       </c>
       <c r="D4" t="n">
         <v>0</v>
       </c>
       <c r="E4" t="n">
-        <v>940</v>
+        <v>11</v>
       </c>
       <c r="F4" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G4" t="n">
-        <v>5970</v>
+        <v>55351</v>
       </c>
       <c r="H4" t="n">
-        <v>62.76</v>
+        <v>17.38</v>
       </c>
       <c r="I4" t="n">
-        <v>99.39034903280067</v>
+        <v>4.771716943329627</v>
       </c>
       <c r="J4" t="n">
-        <v>270.2283705817615</v>
+        <v>3.10253535467032</v>
       </c>
       <c r="K4" t="n">
-        <v>73023.37226727381</v>
+        <v>9.625725626979291</v>
       </c>
       <c r="L4" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M4" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="N4" t="n">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="O4" t="n">
-        <v>19</v>
+        <v>7</v>
       </c>
       <c r="P4" t="n">
-        <v>2103</v>
+        <v>13</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>CONSUMOSTOTAL</t>
+          <t>Available Extra Rooms in Hospital</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
@@ -690,106 +690,106 @@
         </is>
       </c>
       <c r="C5" t="n">
-        <v>9512</v>
+        <v>318438</v>
       </c>
       <c r="D5" t="n">
         <v>0</v>
       </c>
       <c r="E5" t="n">
-        <v>337</v>
+        <v>18</v>
       </c>
       <c r="F5" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="G5" t="n">
-        <v>5513</v>
+        <v>98311</v>
       </c>
       <c r="H5" t="n">
-        <v>57.96</v>
+        <v>30.87</v>
       </c>
       <c r="I5" t="n">
-        <v>101.617535744323</v>
+        <v>3.197627167611905</v>
       </c>
       <c r="J5" t="n">
-        <v>4102.038989216991</v>
+        <v>1.168171427859713</v>
       </c>
       <c r="K5" t="n">
-        <v>16826723.86905636</v>
+        <v>1.3646244848678</v>
       </c>
       <c r="L5" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M5" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="N5" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="O5" t="n">
         <v>4</v>
       </c>
       <c r="P5" t="n">
-        <v>371738</v>
+        <v>24</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>EMPRESASUNICAS_CONSULT</t>
+          <t>Bed Grade</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>int64</t>
+          <t>float64</t>
         </is>
       </c>
       <c r="C6" t="n">
-        <v>9512</v>
+        <v>318325</v>
       </c>
       <c r="D6" t="n">
-        <v>0</v>
+        <v>113</v>
       </c>
       <c r="E6" t="n">
-        <v>241</v>
+        <v>4</v>
       </c>
       <c r="F6" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="G6" t="n">
-        <v>6460</v>
+        <v>123671</v>
       </c>
       <c r="H6" t="n">
-        <v>67.91</v>
+        <v>38.84</v>
       </c>
       <c r="I6" t="n">
-        <v>50.52806980656013</v>
+        <v>2.625806958297338</v>
       </c>
       <c r="J6" t="n">
-        <v>1728.14254228711</v>
+        <v>0.8731458045921731</v>
       </c>
       <c r="K6" t="n">
-        <v>2986476.646462555</v>
+        <v>0.7623835960769133</v>
       </c>
       <c r="L6" t="n">
         <v>1</v>
       </c>
       <c r="M6" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="N6" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="O6" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="P6" t="n">
-        <v>154069</v>
+        <v>4</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>NUM_COMPRAS</t>
+          <t>patientid</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
@@ -798,100 +798,208 @@
         </is>
       </c>
       <c r="C7" t="n">
-        <v>9512</v>
+        <v>318438</v>
       </c>
       <c r="D7" t="n">
         <v>0</v>
       </c>
       <c r="E7" t="n">
-        <v>42</v>
+        <v>92017</v>
       </c>
       <c r="F7" t="n">
-        <v>1</v>
+        <v>66714</v>
       </c>
       <c r="G7" t="n">
-        <v>6264</v>
+        <v>50</v>
       </c>
       <c r="H7" t="n">
-        <v>65.84999999999999</v>
+        <v>0.02</v>
       </c>
       <c r="I7" t="n">
-        <v>2.159062237174096</v>
+        <v>65747.57947229916</v>
       </c>
       <c r="J7" t="n">
-        <v>3.719538090104518</v>
+        <v>37979.93644002391</v>
       </c>
       <c r="K7" t="n">
-        <v>13.83496360373836</v>
+        <v>1442475571.988256</v>
       </c>
       <c r="L7" t="n">
         <v>1</v>
       </c>
       <c r="M7" t="n">
-        <v>1</v>
+        <v>32847</v>
       </c>
       <c r="N7" t="n">
-        <v>1</v>
+        <v>65724.5</v>
       </c>
       <c r="O7" t="n">
-        <v>2</v>
+        <v>98470</v>
       </c>
       <c r="P7" t="n">
-        <v>173</v>
+        <v>131624</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>IMPORTE_COMPRAS</t>
+          <t>City_Code_Patient</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
         <is>
+          <t>float64</t>
+        </is>
+      </c>
+      <c r="C8" t="n">
+        <v>313906</v>
+      </c>
+      <c r="D8" t="n">
+        <v>4532</v>
+      </c>
+      <c r="E8" t="n">
+        <v>37</v>
+      </c>
+      <c r="F8" t="n">
+        <v>8</v>
+      </c>
+      <c r="G8" t="n">
+        <v>124011</v>
+      </c>
+      <c r="H8" t="n">
+        <v>38.94</v>
+      </c>
+      <c r="I8" t="n">
+        <v>7.251858836721821</v>
+      </c>
+      <c r="J8" t="n">
+        <v>4.745265561141458</v>
+      </c>
+      <c r="K8" t="n">
+        <v>22.51754524575516</v>
+      </c>
+      <c r="L8" t="n">
+        <v>1</v>
+      </c>
+      <c r="M8" t="n">
+        <v>4</v>
+      </c>
+      <c r="N8" t="n">
+        <v>8</v>
+      </c>
+      <c r="O8" t="n">
+        <v>8</v>
+      </c>
+      <c r="P8" t="n">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>Visitors with Patient</t>
+        </is>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
           <t>int64</t>
         </is>
       </c>
-      <c r="C8" t="n">
-        <v>9512</v>
-      </c>
-      <c r="D8" t="n">
-        <v>0</v>
-      </c>
-      <c r="E8" t="n">
-        <v>616</v>
-      </c>
-      <c r="F8" t="n">
-        <v>15</v>
-      </c>
-      <c r="G8" t="n">
-        <v>1949</v>
-      </c>
-      <c r="H8" t="n">
-        <v>20.49</v>
-      </c>
-      <c r="I8" t="n">
-        <v>168.1920731707317</v>
-      </c>
-      <c r="J8" t="n">
-        <v>682.5294804255069</v>
-      </c>
-      <c r="K8" t="n">
-        <v>465846.4916499124</v>
-      </c>
-      <c r="L8" t="n">
-        <v>6</v>
-      </c>
-      <c r="M8" t="n">
-        <v>22</v>
-      </c>
-      <c r="N8" t="n">
-        <v>40</v>
-      </c>
-      <c r="O8" t="n">
-        <v>100</v>
-      </c>
-      <c r="P8" t="n">
-        <v>25200</v>
+      <c r="C9" t="n">
+        <v>318438</v>
+      </c>
+      <c r="D9" t="n">
+        <v>0</v>
+      </c>
+      <c r="E9" t="n">
+        <v>28</v>
+      </c>
+      <c r="F9" t="n">
+        <v>2</v>
+      </c>
+      <c r="G9" t="n">
+        <v>138417</v>
+      </c>
+      <c r="H9" t="n">
+        <v>43.47</v>
+      </c>
+      <c r="I9" t="n">
+        <v>3.284099259510485</v>
+      </c>
+      <c r="J9" t="n">
+        <v>1.764061389559201</v>
+      </c>
+      <c r="K9" t="n">
+        <v>3.111912586133538</v>
+      </c>
+      <c r="L9" t="n">
+        <v>0</v>
+      </c>
+      <c r="M9" t="n">
+        <v>2</v>
+      </c>
+      <c r="N9" t="n">
+        <v>3</v>
+      </c>
+      <c r="O9" t="n">
+        <v>4</v>
+      </c>
+      <c r="P9" t="n">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>Admission_Deposit</t>
+        </is>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>float64</t>
+        </is>
+      </c>
+      <c r="C10" t="n">
+        <v>318438</v>
+      </c>
+      <c r="D10" t="n">
+        <v>0</v>
+      </c>
+      <c r="E10" t="n">
+        <v>7300</v>
+      </c>
+      <c r="F10" t="n">
+        <v>4469</v>
+      </c>
+      <c r="G10" t="n">
+        <v>390</v>
+      </c>
+      <c r="H10" t="n">
+        <v>0.12</v>
+      </c>
+      <c r="I10" t="n">
+        <v>4880.749392346391</v>
+      </c>
+      <c r="J10" t="n">
+        <v>1086.776253641621</v>
+      </c>
+      <c r="K10" t="n">
+        <v>1181082.625479318</v>
+      </c>
+      <c r="L10" t="n">
+        <v>1800</v>
+      </c>
+      <c r="M10" t="n">
+        <v>4186</v>
+      </c>
+      <c r="N10" t="n">
+        <v>4741</v>
+      </c>
+      <c r="O10" t="n">
+        <v>5409</v>
+      </c>
+      <c r="P10" t="n">
+        <v>11008</v>
       </c>
     </row>
   </sheetData>
@@ -905,7 +1013,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:H11"/>
+  <dimension ref="A1:H10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -958,7 +1066,7 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>FECHA_REGISTRO</t>
+          <t>Hospital_type_code</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
@@ -967,30 +1075,30 @@
         </is>
       </c>
       <c r="C2" t="n">
-        <v>9512</v>
+        <v>318438</v>
       </c>
       <c r="D2" t="n">
         <v>0</v>
       </c>
       <c r="E2" t="n">
-        <v>9489</v>
+        <v>7</v>
       </c>
       <c r="F2" t="inlineStr">
         <is>
-          <t>1/10/2019 9:50</t>
+          <t>a</t>
         </is>
       </c>
       <c r="G2" t="n">
-        <v>2</v>
+        <v>143425</v>
       </c>
       <c r="H2" t="n">
-        <v>0.02</v>
+        <v>45.04</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>CANAL_REGISTRO</t>
+          <t>Hospital_region_code</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
@@ -999,7 +1107,7 @@
         </is>
       </c>
       <c r="C3" t="n">
-        <v>9512</v>
+        <v>318438</v>
       </c>
       <c r="D3" t="n">
         <v>0</v>
@@ -1009,20 +1117,20 @@
       </c>
       <c r="F3" t="inlineStr">
         <is>
-          <t>Directorios</t>
+          <t>X</t>
         </is>
       </c>
       <c r="G3" t="n">
-        <v>4859</v>
+        <v>133336</v>
       </c>
       <c r="H3" t="n">
-        <v>51.08</v>
+        <v>41.87</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>FECHA_CLIENTE</t>
+          <t>Department</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
@@ -1031,30 +1139,30 @@
         </is>
       </c>
       <c r="C4" t="n">
-        <v>9512</v>
+        <v>318438</v>
       </c>
       <c r="D4" t="n">
         <v>0</v>
       </c>
       <c r="E4" t="n">
-        <v>9477</v>
+        <v>5</v>
       </c>
       <c r="F4" t="inlineStr">
         <is>
-          <t>1/7/2020 11:43</t>
+          <t>gynecology</t>
         </is>
       </c>
       <c r="G4" t="n">
-        <v>2</v>
+        <v>249486</v>
       </c>
       <c r="H4" t="n">
-        <v>0.02</v>
+        <v>78.34999999999999</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>FORMAJURIDICA</t>
+          <t>Ward_Type</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
@@ -1063,30 +1171,30 @@
         </is>
       </c>
       <c r="C5" t="n">
-        <v>9512</v>
+        <v>318438</v>
       </c>
       <c r="D5" t="n">
         <v>0</v>
       </c>
       <c r="E5" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F5" t="inlineStr">
         <is>
-          <t>PERSONA FISICA</t>
+          <t>R</t>
         </is>
       </c>
       <c r="G5" t="n">
-        <v>5600</v>
+        <v>127947</v>
       </c>
       <c r="H5" t="n">
-        <v>58.87</v>
+        <v>40.18</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>SECTOR</t>
+          <t>Ward_Facility_Code</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
@@ -1095,30 +1203,30 @@
         </is>
       </c>
       <c r="C6" t="n">
-        <v>9512</v>
+        <v>318438</v>
       </c>
       <c r="D6" t="n">
         <v>0</v>
       </c>
       <c r="E6" t="n">
-        <v>23</v>
+        <v>6</v>
       </c>
       <c r="F6" t="inlineStr">
         <is>
-          <t>9</t>
+          <t>F</t>
         </is>
       </c>
       <c r="G6" t="n">
-        <v>5600</v>
+        <v>112753</v>
       </c>
       <c r="H6" t="n">
-        <v>58.87</v>
+        <v>35.41</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>DESC_SECTOR</t>
+          <t>Type of Admission</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
@@ -1127,30 +1235,30 @@
         </is>
       </c>
       <c r="C7" t="n">
-        <v>9512</v>
+        <v>318438</v>
       </c>
       <c r="D7" t="n">
         <v>0</v>
       </c>
       <c r="E7" t="n">
-        <v>23</v>
+        <v>3</v>
       </c>
       <c r="F7" t="inlineStr">
         <is>
-          <t>NOSECTOR</t>
+          <t>Trauma</t>
         </is>
       </c>
       <c r="G7" t="n">
-        <v>5600</v>
+        <v>152261</v>
       </c>
       <c r="H7" t="n">
-        <v>58.87</v>
+        <v>47.81</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>ESTADO</t>
+          <t>Severity of Illness</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
@@ -1159,30 +1267,30 @@
         </is>
       </c>
       <c r="C8" t="n">
-        <v>9512</v>
+        <v>318438</v>
       </c>
       <c r="D8" t="n">
         <v>0</v>
       </c>
       <c r="E8" t="n">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="F8" t="inlineStr">
         <is>
-          <t>VIVA</t>
+          <t>Moderate</t>
         </is>
       </c>
       <c r="G8" t="n">
-        <v>5600</v>
+        <v>175843</v>
       </c>
       <c r="H8" t="n">
-        <v>58.87</v>
+        <v>55.22</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>DEPARTAMENTO</t>
+          <t>Age</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
@@ -1191,30 +1299,30 @@
         </is>
       </c>
       <c r="C9" t="n">
-        <v>3912</v>
+        <v>318438</v>
       </c>
       <c r="D9" t="n">
-        <v>5600</v>
+        <v>0</v>
       </c>
       <c r="E9" t="n">
-        <v>31</v>
+        <v>10</v>
       </c>
       <c r="F9" t="inlineStr">
         <is>
-          <t>BOGOTA</t>
+          <t>41-50</t>
         </is>
       </c>
       <c r="G9" t="n">
-        <v>1951</v>
+        <v>63749</v>
       </c>
       <c r="H9" t="n">
-        <v>20.51</v>
+        <v>20.02</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>TAMA•O</t>
+          <t>Stay</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
@@ -1223,56 +1331,24 @@
         </is>
       </c>
       <c r="C10" t="n">
-        <v>3912</v>
+        <v>318438</v>
       </c>
       <c r="D10" t="n">
-        <v>5600</v>
+        <v>0</v>
       </c>
       <c r="E10" t="n">
-        <v>5</v>
+        <v>11</v>
       </c>
       <c r="F10" t="inlineStr">
         <is>
-          <t>MICRO</t>
+          <t>21-30</t>
         </is>
       </c>
       <c r="G10" t="n">
-        <v>1745</v>
+        <v>87491</v>
       </c>
       <c r="H10" t="n">
-        <v>18.35</v>
-      </c>
-    </row>
-    <row r="11">
-      <c r="A11" t="inlineStr">
-        <is>
-          <t>ANTIGUEDAD</t>
-        </is>
-      </c>
-      <c r="B11" t="inlineStr">
-        <is>
-          <t>object</t>
-        </is>
-      </c>
-      <c r="C11" t="n">
-        <v>3912</v>
-      </c>
-      <c r="D11" t="n">
-        <v>5600</v>
-      </c>
-      <c r="E11" t="n">
-        <v>7</v>
-      </c>
-      <c r="F11" t="inlineStr">
-        <is>
-          <t>M†s de 10 A§os</t>
-        </is>
-      </c>
-      <c r="G11" t="n">
-        <v>2491</v>
-      </c>
-      <c r="H11" t="n">
-        <v>26.19</v>
+        <v>27.48</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Actualización sin pestañas y revisados gráficos de datetime
</commit_message>
<xml_diff>
--- a/summary.xlsx
+++ b/summary.xlsx
@@ -8,8 +8,9 @@
   </bookViews>
   <sheets>
     <sheet name="Numeric" sheetId="1" state="visible" r:id="rId1"/>
-    <sheet name="Categorical" sheetId="2" state="visible" r:id="rId2"/>
-    <sheet name="Datetime" sheetId="3" state="visible" r:id="rId3"/>
+    <sheet name="Binary" sheetId="2" state="visible" r:id="rId2"/>
+    <sheet name="Categorical" sheetId="3" state="visible" r:id="rId3"/>
+    <sheet name="Datetime" sheetId="4" state="visible" r:id="rId4"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -427,7 +428,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:P3"/>
+  <dimension ref="A1:P7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -529,7 +530,7 @@
         </is>
       </c>
       <c r="C2" t="n">
-        <v>20537</v>
+        <v>9512</v>
       </c>
       <c r="D2" t="n">
         <v>0</v>
@@ -538,34 +539,34 @@
         <v>9512</v>
       </c>
       <c r="F2" t="n">
-        <v>8125558</v>
+        <v>6308943</v>
       </c>
       <c r="G2" t="n">
-        <v>173</v>
+        <v>1</v>
       </c>
       <c r="H2" t="n">
-        <v>0.84</v>
+        <v>0.01</v>
       </c>
       <c r="I2" t="n">
-        <v>8062243.787408093</v>
+        <v>8210750.886459209</v>
       </c>
       <c r="J2" t="n">
-        <v>1084786.334184386</v>
+        <v>1099345.770765004</v>
       </c>
       <c r="K2" t="n">
-        <v>1176761390833.198</v>
+        <v>1208561123698.9</v>
       </c>
       <c r="L2" t="n">
         <v>6308943</v>
       </c>
       <c r="M2" t="n">
-        <v>7100681</v>
+        <v>7227208.75</v>
       </c>
       <c r="N2" t="n">
-        <v>7997236</v>
+        <v>8342317</v>
       </c>
       <c r="O2" t="n">
-        <v>9012504</v>
+        <v>9160217.75</v>
       </c>
       <c r="P2" t="n">
         <v>9987369</v>
@@ -574,7 +575,7 @@
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>IMPORTE</t>
+          <t>DIASCLIENTE</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
@@ -583,46 +584,262 @@
         </is>
       </c>
       <c r="C3" t="n">
-        <v>20537</v>
+        <v>9512</v>
       </c>
       <c r="D3" t="n">
         <v>0</v>
       </c>
       <c r="E3" t="n">
-        <v>48</v>
+        <v>940</v>
       </c>
       <c r="F3" t="n">
+        <v>0</v>
+      </c>
+      <c r="G3" t="n">
+        <v>5970</v>
+      </c>
+      <c r="H3" t="n">
+        <v>62.76</v>
+      </c>
+      <c r="I3" t="n">
+        <v>99.39034903280067</v>
+      </c>
+      <c r="J3" t="n">
+        <v>270.2283705817615</v>
+      </c>
+      <c r="K3" t="n">
+        <v>73023.37226727381</v>
+      </c>
+      <c r="L3" t="n">
+        <v>0</v>
+      </c>
+      <c r="M3" t="n">
+        <v>0</v>
+      </c>
+      <c r="N3" t="n">
+        <v>0</v>
+      </c>
+      <c r="O3" t="n">
+        <v>19</v>
+      </c>
+      <c r="P3" t="n">
+        <v>2103</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>CONSUMOSTOTAL</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>numeric</t>
+        </is>
+      </c>
+      <c r="C4" t="n">
+        <v>9512</v>
+      </c>
+      <c r="D4" t="n">
+        <v>0</v>
+      </c>
+      <c r="E4" t="n">
+        <v>337</v>
+      </c>
+      <c r="F4" t="n">
+        <v>1</v>
+      </c>
+      <c r="G4" t="n">
+        <v>5513</v>
+      </c>
+      <c r="H4" t="n">
+        <v>57.96</v>
+      </c>
+      <c r="I4" t="n">
+        <v>101.617535744323</v>
+      </c>
+      <c r="J4" t="n">
+        <v>4102.038989216991</v>
+      </c>
+      <c r="K4" t="n">
+        <v>16826723.86905636</v>
+      </c>
+      <c r="L4" t="n">
+        <v>1</v>
+      </c>
+      <c r="M4" t="n">
+        <v>1</v>
+      </c>
+      <c r="N4" t="n">
+        <v>1</v>
+      </c>
+      <c r="O4" t="n">
+        <v>4</v>
+      </c>
+      <c r="P4" t="n">
+        <v>371738</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>EMPRESASUNICAS_CONSULT</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>numeric</t>
+        </is>
+      </c>
+      <c r="C5" t="n">
+        <v>9512</v>
+      </c>
+      <c r="D5" t="n">
+        <v>0</v>
+      </c>
+      <c r="E5" t="n">
+        <v>241</v>
+      </c>
+      <c r="F5" t="n">
+        <v>1</v>
+      </c>
+      <c r="G5" t="n">
+        <v>6460</v>
+      </c>
+      <c r="H5" t="n">
+        <v>67.91</v>
+      </c>
+      <c r="I5" t="n">
+        <v>50.52806980656013</v>
+      </c>
+      <c r="J5" t="n">
+        <v>1728.14254228711</v>
+      </c>
+      <c r="K5" t="n">
+        <v>2986476.646462555</v>
+      </c>
+      <c r="L5" t="n">
+        <v>1</v>
+      </c>
+      <c r="M5" t="n">
+        <v>1</v>
+      </c>
+      <c r="N5" t="n">
+        <v>1</v>
+      </c>
+      <c r="O5" t="n">
+        <v>2</v>
+      </c>
+      <c r="P5" t="n">
+        <v>154069</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>NUM_COMPRAS</t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>numeric</t>
+        </is>
+      </c>
+      <c r="C6" t="n">
+        <v>9512</v>
+      </c>
+      <c r="D6" t="n">
+        <v>0</v>
+      </c>
+      <c r="E6" t="n">
+        <v>42</v>
+      </c>
+      <c r="F6" t="n">
+        <v>1</v>
+      </c>
+      <c r="G6" t="n">
+        <v>6264</v>
+      </c>
+      <c r="H6" t="n">
+        <v>65.84999999999999</v>
+      </c>
+      <c r="I6" t="n">
+        <v>2.159062237174096</v>
+      </c>
+      <c r="J6" t="n">
+        <v>3.719538090104518</v>
+      </c>
+      <c r="K6" t="n">
+        <v>13.83496360373836</v>
+      </c>
+      <c r="L6" t="n">
+        <v>1</v>
+      </c>
+      <c r="M6" t="n">
+        <v>1</v>
+      </c>
+      <c r="N6" t="n">
+        <v>1</v>
+      </c>
+      <c r="O6" t="n">
+        <v>2</v>
+      </c>
+      <c r="P6" t="n">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>IMPORTE_COMPRAS</t>
+        </is>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>numeric</t>
+        </is>
+      </c>
+      <c r="C7" t="n">
+        <v>9512</v>
+      </c>
+      <c r="D7" t="n">
+        <v>0</v>
+      </c>
+      <c r="E7" t="n">
+        <v>616</v>
+      </c>
+      <c r="F7" t="n">
         <v>15</v>
       </c>
-      <c r="G3" t="n">
-        <v>4844</v>
-      </c>
-      <c r="H3" t="n">
-        <v>23.59</v>
-      </c>
-      <c r="I3" t="n">
-        <v>77.90052101085845</v>
-      </c>
-      <c r="J3" t="n">
-        <v>200.6320422788847</v>
-      </c>
-      <c r="K3" t="n">
-        <v>40253.21638899616</v>
-      </c>
-      <c r="L3" t="n">
+      <c r="G7" t="n">
+        <v>1949</v>
+      </c>
+      <c r="H7" t="n">
+        <v>20.49</v>
+      </c>
+      <c r="I7" t="n">
+        <v>168.1920731707317</v>
+      </c>
+      <c r="J7" t="n">
+        <v>682.5294804255069</v>
+      </c>
+      <c r="K7" t="n">
+        <v>465846.4916499124</v>
+      </c>
+      <c r="L7" t="n">
         <v>6</v>
       </c>
-      <c r="M3" t="n">
-        <v>15</v>
-      </c>
-      <c r="N3" t="n">
-        <v>35</v>
-      </c>
-      <c r="O3" t="n">
-        <v>65</v>
-      </c>
-      <c r="P3" t="n">
-        <v>4875</v>
+      <c r="M7" t="n">
+        <v>22</v>
+      </c>
+      <c r="N7" t="n">
+        <v>40</v>
+      </c>
+      <c r="O7" t="n">
+        <v>100</v>
+      </c>
+      <c r="P7" t="n">
+        <v>25200</v>
       </c>
     </row>
   </sheetData>
@@ -636,7 +853,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:H3"/>
+  <dimension ref="A1:H2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -689,65 +906,31 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>PRODUCTOCOMPRADO</t>
+          <t>CLIENTEPORCAMPA•AEMAIL</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>categorical</t>
+          <t>binary</t>
         </is>
       </c>
       <c r="C2" t="n">
-        <v>20537</v>
+        <v>9512</v>
       </c>
       <c r="D2" t="n">
         <v>0</v>
       </c>
       <c r="E2" t="n">
-        <v>3</v>
-      </c>
-      <c r="F2" t="inlineStr">
-        <is>
-          <t>VP Informe</t>
-        </is>
+        <v>2</v>
+      </c>
+      <c r="F2" t="n">
+        <v>0</v>
       </c>
       <c r="G2" t="n">
-        <v>18020</v>
+        <v>8717</v>
       </c>
       <c r="H2" t="n">
-        <v>87.73999999999999</v>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" t="inlineStr">
-        <is>
-          <t>CANALVENTA</t>
-        </is>
-      </c>
-      <c r="B3" t="inlineStr">
-        <is>
-          <t>categorical</t>
-        </is>
-      </c>
-      <c r="C3" t="n">
-        <v>20537</v>
-      </c>
-      <c r="D3" t="n">
-        <v>0</v>
-      </c>
-      <c r="E3" t="n">
-        <v>2</v>
-      </c>
-      <c r="F3" t="inlineStr">
-        <is>
-          <t>WEB</t>
-        </is>
-      </c>
-      <c r="G3" t="n">
-        <v>18478</v>
-      </c>
-      <c r="H3" t="n">
-        <v>89.97</v>
+        <v>91.64</v>
       </c>
     </row>
   </sheetData>
@@ -761,7 +944,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G2"/>
+  <dimension ref="A1:H9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -797,43 +980,391 @@
       </c>
       <c r="F1" s="1" t="inlineStr">
         <is>
-          <t>Min</t>
+          <t>Top</t>
         </is>
       </c>
       <c r="G1" s="1" t="inlineStr">
         <is>
-          <t>Max</t>
+          <t>Freq Top</t>
+        </is>
+      </c>
+      <c r="H1" s="1" t="inlineStr">
+        <is>
+          <t>% Top</t>
         </is>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>FECHAVENTA</t>
+          <t>CANAL_REGISTRO</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
+          <t>categorical</t>
+        </is>
+      </c>
+      <c r="C2" t="n">
+        <v>9512</v>
+      </c>
+      <c r="D2" t="n">
+        <v>0</v>
+      </c>
+      <c r="E2" t="n">
+        <v>3</v>
+      </c>
+      <c r="F2" t="inlineStr">
+        <is>
+          <t>Directorios</t>
+        </is>
+      </c>
+      <c r="G2" t="n">
+        <v>4859</v>
+      </c>
+      <c r="H2" t="n">
+        <v>51.08</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>FORMAJURIDICA</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>categorical</t>
+        </is>
+      </c>
+      <c r="C3" t="n">
+        <v>9512</v>
+      </c>
+      <c r="D3" t="n">
+        <v>0</v>
+      </c>
+      <c r="E3" t="n">
+        <v>7</v>
+      </c>
+      <c r="F3" t="inlineStr">
+        <is>
+          <t>PERSONA FISICA</t>
+        </is>
+      </c>
+      <c r="G3" t="n">
+        <v>5600</v>
+      </c>
+      <c r="H3" t="n">
+        <v>58.87</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>SECTOR</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>categorical</t>
+        </is>
+      </c>
+      <c r="C4" t="n">
+        <v>9512</v>
+      </c>
+      <c r="D4" t="n">
+        <v>0</v>
+      </c>
+      <c r="E4" t="n">
+        <v>23</v>
+      </c>
+      <c r="F4" t="inlineStr">
+        <is>
+          <t>9</t>
+        </is>
+      </c>
+      <c r="G4" t="n">
+        <v>5600</v>
+      </c>
+      <c r="H4" t="n">
+        <v>58.87</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>DESC_SECTOR</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>categorical</t>
+        </is>
+      </c>
+      <c r="C5" t="n">
+        <v>9512</v>
+      </c>
+      <c r="D5" t="n">
+        <v>0</v>
+      </c>
+      <c r="E5" t="n">
+        <v>23</v>
+      </c>
+      <c r="F5" t="inlineStr">
+        <is>
+          <t>NOSECTOR</t>
+        </is>
+      </c>
+      <c r="G5" t="n">
+        <v>5600</v>
+      </c>
+      <c r="H5" t="n">
+        <v>58.87</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>ESTADO</t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>categorical</t>
+        </is>
+      </c>
+      <c r="C6" t="n">
+        <v>9512</v>
+      </c>
+      <c r="D6" t="n">
+        <v>0</v>
+      </c>
+      <c r="E6" t="n">
+        <v>5</v>
+      </c>
+      <c r="F6" t="inlineStr">
+        <is>
+          <t>VIVA</t>
+        </is>
+      </c>
+      <c r="G6" t="n">
+        <v>5600</v>
+      </c>
+      <c r="H6" t="n">
+        <v>58.87</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>DEPARTAMENTO</t>
+        </is>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>categorical</t>
+        </is>
+      </c>
+      <c r="C7" t="n">
+        <v>3912</v>
+      </c>
+      <c r="D7" t="n">
+        <v>5600</v>
+      </c>
+      <c r="E7" t="n">
+        <v>31</v>
+      </c>
+      <c r="F7" t="inlineStr">
+        <is>
+          <t>BOGOTA</t>
+        </is>
+      </c>
+      <c r="G7" t="n">
+        <v>1951</v>
+      </c>
+      <c r="H7" t="n">
+        <v>20.51</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>TAMA•O</t>
+        </is>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>categorical</t>
+        </is>
+      </c>
+      <c r="C8" t="n">
+        <v>3912</v>
+      </c>
+      <c r="D8" t="n">
+        <v>5600</v>
+      </c>
+      <c r="E8" t="n">
+        <v>5</v>
+      </c>
+      <c r="F8" t="inlineStr">
+        <is>
+          <t>MICRO</t>
+        </is>
+      </c>
+      <c r="G8" t="n">
+        <v>1745</v>
+      </c>
+      <c r="H8" t="n">
+        <v>18.35</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>ANTIGUEDAD</t>
+        </is>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>categorical</t>
+        </is>
+      </c>
+      <c r="C9" t="n">
+        <v>3912</v>
+      </c>
+      <c r="D9" t="n">
+        <v>5600</v>
+      </c>
+      <c r="E9" t="n">
+        <v>7</v>
+      </c>
+      <c r="F9" t="inlineStr">
+        <is>
+          <t>M†s de 10 A§os</t>
+        </is>
+      </c>
+      <c r="G9" t="n">
+        <v>2491</v>
+      </c>
+      <c r="H9" t="n">
+        <v>26.19</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:G3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>Variable</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>Type</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>Non-null</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
+          <t>Nulls</t>
+        </is>
+      </c>
+      <c r="E1" s="1" t="inlineStr">
+        <is>
+          <t>Unique</t>
+        </is>
+      </c>
+      <c r="F1" s="1" t="inlineStr">
+        <is>
+          <t>Min</t>
+        </is>
+      </c>
+      <c r="G1" s="1" t="inlineStr">
+        <is>
+          <t>Max</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>FECHA_REGISTRO</t>
+        </is>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
           <t>datetime</t>
         </is>
       </c>
       <c r="C2" t="n">
-        <v>20537</v>
+        <v>9512</v>
       </c>
       <c r="D2" t="n">
         <v>0</v>
       </c>
       <c r="E2" t="n">
-        <v>2250</v>
+        <v>9489</v>
       </c>
       <c r="F2" t="inlineStr">
         <is>
-          <t>1/1/2020 0:00</t>
+          <t>1/10/2017 11:42</t>
         </is>
       </c>
       <c r="G2" t="inlineStr">
         <is>
-          <t>9/9/2022 0:00</t>
+          <t>9/9/2022 9:48</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>FECHA_CLIENTE</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>datetime</t>
+        </is>
+      </c>
+      <c r="C3" t="n">
+        <v>9512</v>
+      </c>
+      <c r="D3" t="n">
+        <v>0</v>
+      </c>
+      <c r="E3" t="n">
+        <v>9477</v>
+      </c>
+      <c r="F3" t="inlineStr">
+        <is>
+          <t>1/1/2020 16:24</t>
+        </is>
+      </c>
+      <c r="G3" t="inlineStr">
+        <is>
+          <t>9/9/2022 4:05</t>
         </is>
       </c>
     </row>

</xml_diff>